<commit_message>
Correccion en signo de metrica NCH y pequeño agregado en Metricas campaña 3.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/Metricas campaña 3.xlsx
+++ b/Documentacion/Metricas campaña 3.xlsx
@@ -1394,7 +1394,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1437,9 +1437,9 @@
         <f>SUM(Hoja2!E2:E32)</f>
         <v>1818</v>
       </c>
-      <c r="E3" s="13">
-        <f>Hoja5!C1</f>
-        <v>6.1606160616061603</v>
+      <c r="E3" s="1">
+        <f>ROUND(Hoja5!C1,2)</f>
+        <v>6.16</v>
       </c>
       <c r="F3" s="23">
         <f>SUM(Hoja6!I2:I32)</f>
@@ -1458,8 +1458,8 @@
         <v>1961</v>
       </c>
       <c r="E4" s="1">
-        <f>Hoja5!C2</f>
-        <v>4.9464558898521167</v>
+        <f>ROUND(Hoja5!C2,2)</f>
+        <v>4.95</v>
       </c>
       <c r="F4" s="3">
         <f>SUM(Hoja6!I33:I63)</f>
@@ -1478,8 +1478,8 @@
         <v>1817</v>
       </c>
       <c r="E5" s="1">
-        <f>Hoja5!C3</f>
-        <v>5.9988992845349474</v>
+        <f>ROUND(Hoja5!C3,2)</f>
+        <v>6</v>
       </c>
       <c r="F5" s="3">
         <f>SUM(Hoja6!I64:I94)</f>
@@ -1497,9 +1497,9 @@
         <f>SUM(Hoja2!E95:E125)</f>
         <v>1863</v>
       </c>
-      <c r="E6" s="5">
-        <f>Hoja5!C4</f>
-        <v>4.8845947396672038</v>
+      <c r="E6" s="1">
+        <f>ROUND(Hoja5!C4,2)</f>
+        <v>4.88</v>
       </c>
       <c r="F6" s="6">
         <f>SUM(Hoja6!I95:I125)</f>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="E9" s="28">
         <f>AVERAGE(E3:E4)</f>
-        <v>5.5535359757291385</v>
+        <v>5.5549999999999997</v>
       </c>
       <c r="F9" s="29">
         <f>SUM(F3:F4)</f>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="E12" s="28">
         <f>AVERAGE(E3:E6)</f>
-        <v>5.4976414939151068</v>
+        <v>5.4974999999999996</v>
       </c>
       <c r="F12" s="29">
         <f>SUM(F3:F6)</f>
@@ -1578,7 +1578,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="D3 D4:D6" formulaRange="1"/>
-    <ignoredError sqref="E9 E12" formula="1"/>
+    <ignoredError sqref="E12" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>